<commit_message>
folder copying and deletion and column renaming bugfixes
- fixed old cogntiive test data not being deleted
- fixed cogntiive test data not being copied in all_backbone_data
- fixed remids that oculd nto be matched being forgotten (now rpinted to log)
- fixed script so it can now deal with renaming of the psytoolkit column names
- created most recent version of data collection progress update
</commit_message>
<xml_diff>
--- a/information/2025-11-10_Target_Sample_Size_Projects.xlsx
+++ b/information/2025-11-10_Target_Sample_Size_Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13EFB07-F1FF-42CC-99F9-D1FDB7B2178B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C0DF35-D4C3-4182-8720-F3DDC0123A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5715" yWindow="3375" windowWidth="19185" windowHeight="10065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>p2</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>p6_children</t>
+  </si>
+  <si>
+    <t>p6_infants</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC51527D-4322-4172-88D8-18B26E439C2C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,41 +529,46 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>80</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>400</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>130</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prokject-specific demography plots, target sample size fix, timeline fix
implement visualization of demographic data per project
updated target  sample sizes
fixed issue with imissing submit dates for timeline plot
</commit_message>
<xml_diff>
--- a/information/2025-11-10_Target_Sample_Size_Projects.xlsx
+++ b/information/2025-11-10_Target_Sample_Size_Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Wilken Arbeitsordner\Clinical_Backbone_RU5389\information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C0DF35-D4C3-4182-8720-F3DDC0123A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1836EE8B-BF94-44DA-AB5A-BA18BAECC95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="3375" windowWidth="19185" windowHeight="10065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6750" yWindow="4410" windowWidth="19185" windowHeight="10065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +415,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>